<commit_message>
edit button anvar aka
</commit_message>
<xml_diff>
--- a/monitoring.xlsx
+++ b/monitoring.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="24">
   <si>
     <t>Developers</t>
   </si>
@@ -27,21 +27,18 @@
     <t>user_id</t>
   </si>
   <si>
-    <t>Umarjonov Ulug'bek</t>
-  </si>
-  <si>
     <t xml:space="preserve">49257001: </t>
   </si>
   <si>
+    <t>.</t>
+  </si>
+  <si>
     <t>Tulaboyev Zafar</t>
   </si>
   <si>
     <t xml:space="preserve">10414033: </t>
   </si>
   <si>
-    <t>Sabina Sobirovna</t>
-  </si>
-  <si>
     <t>2111796525:</t>
   </si>
   <si>
@@ -51,7 +48,7 @@
     <t>328628941:</t>
   </si>
   <si>
-    <t>Sharifjon Mo`minov</t>
+    <t>Keldi: 13:35:24 Ketdi: 13:35:37</t>
   </si>
   <si>
     <t>5172746353:</t>
@@ -69,26 +66,51 @@
     <t>524697244:</t>
   </si>
   <si>
-    <t>Сматуллаев Ербол</t>
-  </si>
-  <si>
     <t>322626456:</t>
   </si>
   <si>
-    <t>.</t>
+    <t>Smatullayev Erbol</t>
+  </si>
+  <si>
+    <t>Yo‘ldoshev Bobur</t>
+  </si>
+  <si>
+    <t>Sharifjon Mo‘minov</t>
+  </si>
+  <si>
+    <t>Maxmudova Durdona</t>
+  </si>
+  <si>
+    <t>Sobirova Sabina</t>
+  </si>
+  <si>
+    <t>Nazaraliyev Jahongir</t>
+  </si>
+  <si>
+    <t>1336680858:</t>
+  </si>
+  <si>
+    <t>1755017200:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,8 +133,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -415,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF9"/>
+  <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,790 +553,987 @@
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
+      <c r="A2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Q2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="R2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="S2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="U2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="V2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="W2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="X2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Y2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Z2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AA2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AB2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AC2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AD2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AE2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AF2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="O3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Q3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="R3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="S3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="T3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="U3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="V3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="W3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="X3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Y3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Z3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AA3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AB3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AC3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AD3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AE3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AF3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="O4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="P4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Q4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="R4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="S4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="T4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="U4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="V4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="W4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="X4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Y4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Z4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AA4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AB4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AC4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AD4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AE4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AF4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
+      <c r="A5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="N5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="O5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="P5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Q5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="R5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="S5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="T5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="U5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="V5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="W5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="X5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Y5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Z5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AA5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AB5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AC5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AD5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AE5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AF5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>213</v>
-      </c>
-      <c r="D6">
-        <v>123123</v>
-      </c>
-      <c r="E6">
-        <v>123123</v>
-      </c>
-      <c r="F6">
-        <v>124</v>
-      </c>
-      <c r="G6">
-        <v>123125123</v>
-      </c>
-      <c r="H6">
-        <v>123</v>
-      </c>
-      <c r="I6">
-        <v>12313</v>
-      </c>
-      <c r="J6">
-        <v>1231</v>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>3</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="M6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="N6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="O6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="P6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Q6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="R6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="S6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="T6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="U6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="V6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="W6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="X6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Y6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Z6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AA6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AB6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AC6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AD6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AE6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AF6" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
+      <c r="A7" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="K7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="M7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="N7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="O7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="P7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Q7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="R7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="S7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="T7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="U7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="V7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="W7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="X7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Y7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Z7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AA7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AB7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AC7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AD7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AE7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AF7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
+      <c r="A8" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="M8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="N8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="O8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Q8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="S8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="T8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="U8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="V8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="W8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="X8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Y8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Z8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AA8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AB8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AC8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AD8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AE8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AF8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>16</v>
+      <c r="A9" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="M9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="N9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="O9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="P9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Q9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="R9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="S9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="T9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="U9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="V9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="W9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="X9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Y9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="Z9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AA9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AB9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AC9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AD9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AE9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AF9" t="s">
-        <v>18</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="15" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>3</v>
+      </c>
+      <c r="R10" t="s">
+        <v>3</v>
+      </c>
+      <c r="S10" t="s">
+        <v>3</v>
+      </c>
+      <c r="T10" t="s">
+        <v>3</v>
+      </c>
+      <c r="U10" t="s">
+        <v>3</v>
+      </c>
+      <c r="V10" t="s">
+        <v>3</v>
+      </c>
+      <c r="W10" t="s">
+        <v>3</v>
+      </c>
+      <c r="X10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="15" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>3</v>
+      </c>
+      <c r="R11" t="s">
+        <v>3</v>
+      </c>
+      <c r="S11" t="s">
+        <v>3</v>
+      </c>
+      <c r="T11" t="s">
+        <v>3</v>
+      </c>
+      <c r="U11" t="s">
+        <v>3</v>
+      </c>
+      <c r="V11" t="s">
+        <v>3</v>
+      </c>
+      <c r="W11" t="s">
+        <v>3</v>
+      </c>
+      <c r="X11" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>